<commit_message>
Add test for timed transitions and junction residual syntax
</commit_message>
<xml_diff>
--- a/tests/timed_test_indirect_framework.xlsx
+++ b/tests/timed_test_indirect_framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB65BC5-6E6F-4D61-B06A-DCA918E5EC4C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53BF8A5-2894-4A49-AC37-85FAEADA25AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="3525" windowWidth="26730" windowHeight="16305" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="5565" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -338,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -530,6 +533,9 @@
   </si>
   <si>
     <t>Initial delay</t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1463,7 @@
   <dimension ref="A1:OH398"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3076,7 +3082,7 @@
         <v>45</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:398" x14ac:dyDescent="0.25">

</xml_diff>